<commit_message>
add MI healthy climate plan
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
+++ b/InputData/ctrl-settings/GRA/Government Revenue Accounting.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/gra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Michigan\MI-EPS\InputData\ctrl-settings\GRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE535FE-2280-DF4E-AC32-9EA66AB8F26C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B1E66-14B6-435A-A4F8-8D680ED0C44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2680" windowWidth="25660" windowHeight="13520" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="70" yWindow="110" windowWidth="15950" windowHeight="13090" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9200" yWindow="660" windowWidth="15950" windowHeight="13090" activeTab="1" xr2:uid="{EBEF7364-D6A1-450C-A98F-6C9C4F55F73F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="78">
   <si>
     <t>GRA Government Revenue Accounting</t>
   </si>
@@ -260,6 +261,42 @@
   </si>
   <si>
     <t>Government revenue handling is one of the design decisions a model user should make</t>
+  </si>
+  <si>
+    <t>GRA for Carbon Tax Revenue[household taxes] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Fuel Tax Revenue[household taxes] = 5</t>
+  </si>
+  <si>
+    <t>GRA for EV Subsidy[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Electricity Generation Subsidies[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Electricity Capacity Construction Subsidies[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Distributed Solar Subsidy[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Fuel Subsidies[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for National Debt Interest[regular spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for National Debt Interest[household taxes] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Remaining Government Cash Flow Changes[regular spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Remaining Government Cash Flow Changes[deficit spending] = 5</t>
+  </si>
+  <si>
+    <t>GRA for Remaining Government Cash Flow Changes[household taxes] = 5</t>
   </si>
 </sst>
 </file>
@@ -708,16 +745,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="80.83203125" customWidth="1"/>
+    <col min="1" max="1" width="69.6328125" customWidth="1"/>
+    <col min="2" max="2" width="80.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +766,7 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -733,72 +774,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -806,7 +847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -814,7 +855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -822,7 +863,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>4</v>
       </c>
@@ -830,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -838,116 +879,176 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -964,13 +1065,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -978,7 +1080,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -987,7 +1089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -995,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1003,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1032,13 +1134,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1046,7 +1149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1055,7 +1158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1063,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +1174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1079,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1100,36 +1203,39 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>
@@ -1139,7 +1245,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>46</v>
       </c>
@@ -1159,7 +1265,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1167,19 +1273,19 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1219,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1259,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1279,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1299,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1319,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1339,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>52</v>
       </c>
@@ -1349,12 +1455,12 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
@@ -1374,7 +1480,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1384,22 +1490,22 @@
       </c>
       <c r="C22" s="10">
         <f t="shared" ref="C22:F22" si="0">IFERROR(C8/SUM($B8:$F8),1/COUNT($B8:$F8))</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="D22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="E22" s="10">
         <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1424,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1449,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1474,7 +1580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1499,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1524,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1574,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1616,13 +1722,16 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1630,7 +1739,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1639,15 +1748,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1655,15 +1764,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1684,13 +1793,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1698,7 +1808,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1707,7 +1817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1715,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1723,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1731,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1752,13 +1862,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1766,7 +1877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1775,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1783,7 +1894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1791,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1799,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1820,13 +1931,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1946,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1843,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1851,7 +1963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1859,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1867,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1888,13 +2000,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1902,7 +2015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1911,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1919,7 +2032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1927,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1935,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1956,13 +2069,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1970,7 +2084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1979,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1987,7 +2101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1995,7 +2109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -2024,13 +2138,14 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -2038,7 +2153,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2047,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2055,7 +2170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2063,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2071,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>64</v>
       </c>

</xml_diff>